<commit_message>
Se agrego el estado civil de las personas como tambien si es empleado permanentes o temporal
</commit_message>
<xml_diff>
--- a/base de datos.xlsx
+++ b/base de datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\NUEVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C79D5BC-2615-4E70-BA00-F07E92C42BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95AE119-559D-42C6-8A73-85B71276604B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6DB1B80C-C695-4F54-8503-2EE8A0A1B1CC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
   <si>
     <t>N°</t>
   </si>
@@ -55,6 +55,27 @@
   </si>
   <si>
     <t>EDAD</t>
+  </si>
+  <si>
+    <t>EMPLEADO</t>
+  </si>
+  <si>
+    <t>PERMANENTE</t>
+  </si>
+  <si>
+    <t>TEMPORAL</t>
+  </si>
+  <si>
+    <t>ESTADO CIVIL</t>
+  </si>
+  <si>
+    <t>CASADO</t>
+  </si>
+  <si>
+    <t>SOLTERO</t>
+  </si>
+  <si>
+    <t>DIVORCIADO</t>
   </si>
 </sst>
 </file>
@@ -423,15 +444,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23F2324-5568-4370-861B-EFEF0836E94C}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -441,8 +466,14 @@
       <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -452,8 +483,14 @@
       <c r="C2" s="2">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -463,8 +500,14 @@
       <c r="C3" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -474,8 +517,14 @@
       <c r="C4" s="2">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -485,8 +534,14 @@
       <c r="C5" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -496,8 +551,14 @@
       <c r="C6" s="2">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -507,8 +568,14 @@
       <c r="C7" s="2">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -518,8 +585,14 @@
       <c r="C8" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -529,8 +602,14 @@
       <c r="C9" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -540,8 +619,14 @@
       <c r="C10" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -550,6 +635,12 @@
       </c>
       <c r="C11" s="2">
         <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Esta es la nueva prueba del comando para hacer un git add y un commit al mismo tiempo
</commit_message>
<xml_diff>
--- a/base de datos.xlsx
+++ b/base de datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\NUEVA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95AE119-559D-42C6-8A73-85B71276604B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F313573-18BC-4FD3-8712-B0492AD3F6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6DB1B80C-C695-4F54-8503-2EE8A0A1B1CC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
   <si>
     <t>N°</t>
   </si>
@@ -76,6 +76,30 @@
   </si>
   <si>
     <t>DIVORCIADO</t>
+  </si>
+  <si>
+    <t>REGALO</t>
+  </si>
+  <si>
+    <t>FLORES</t>
+  </si>
+  <si>
+    <t>GASEOSA</t>
+  </si>
+  <si>
+    <t>PERRO</t>
+  </si>
+  <si>
+    <t>ESCOBA</t>
+  </si>
+  <si>
+    <t>ROPA</t>
+  </si>
+  <si>
+    <t>CALCETINES</t>
+  </si>
+  <si>
+    <t>ZAPATOS</t>
   </si>
 </sst>
 </file>
@@ -444,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23F2324-5568-4370-861B-EFEF0836E94C}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,7 +480,7 @@
     <col min="5" max="5" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -472,8 +496,11 @@
       <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -489,8 +516,11 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -506,8 +536,11 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -523,8 +556,11 @@
       <c r="E4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -540,8 +576,11 @@
       <c r="E5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -557,8 +596,11 @@
       <c r="E6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -574,8 +616,11 @@
       <c r="E7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -591,8 +636,11 @@
       <c r="E8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -608,8 +656,11 @@
       <c r="E9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -625,8 +676,11 @@
       <c r="E10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -641,6 +695,9 @@
       </c>
       <c r="E11" t="s">
         <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>